<commit_message>
img2tile based on colour histograms vs labeled images
</commit_message>
<xml_diff>
--- a/maps/tilemaps/Braunschweig_SQ.xlsx
+++ b/maps/tilemaps/Braunschweig_SQ.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="3">
-  <si>
-    <t>G</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="4">
   <si>
     <t>B</t>
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -82,10 +85,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -406,274 +409,274 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1" max="15" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,45 +687,45 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -731,72 +734,72 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>0</v>
@@ -805,51 +808,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+    <row r="10" spans="1:14" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,78 +860,78 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+    <row r="12" spans="1:14" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>0</v>
@@ -937,36 +940,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+    <row r="13" spans="1:14" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>0</v>
@@ -975,18 +978,18 @@
         <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" ht="45.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -995,34 +998,34 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classify by pixel histograms
</commit_message>
<xml_diff>
--- a/maps/tilemaps/Braunschweig_SQ.xlsx
+++ b/maps/tilemaps/Braunschweig_SQ.xlsx
@@ -14,18 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="5">
+  <si>
+    <t>L</t>
+  </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -426,34 +429,34 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1">
@@ -461,13 +464,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -476,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -494,24 +497,24 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -520,10 +523,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>0</v>
@@ -538,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>2</v>
@@ -549,20 +552,20 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G4" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,24 +585,24 @@
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -617,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>0</v>
@@ -643,13 +646,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>0</v>
@@ -658,22 +661,22 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1">
@@ -684,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -699,69 +702,69 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1">
@@ -769,16 +772,16 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
@@ -813,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -840,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>0</v>
@@ -849,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1">
@@ -860,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>0</v>
@@ -869,13 +872,13 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>0</v>
@@ -884,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>0</v>
@@ -901,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -913,57 +916,57 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>0</v>
@@ -978,18 +981,18 @@
         <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -998,34 +1001,34 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>